<commit_message>
add final resource for kindlegen
</commit_message>
<xml_diff>
--- a/input/im_workflow/definition.xlsx
+++ b/input/im_workflow/definition.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="20" windowWidth="28800" windowHeight="16860" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="27795" windowHeight="13110" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="macro" sheetId="4" r:id="rId1"/>
     <sheet name="database" sheetId="1" r:id="rId2"/>
     <sheet name="main" sheetId="8" r:id="rId3"/>
     <sheet name="message" sheetId="7" r:id="rId4"/>
-    <sheet name="screen-001" sheetId="5" r:id="rId5"/>
+    <sheet name="screen-0001" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="95">
   <si>
     <t>project_name</t>
   </si>
@@ -304,9 +299,6 @@
     <t>CODE</t>
   </si>
   <si>
-    <t>UID</t>
-  </si>
-  <si>
     <t>Commodity purchase - TERASOLUNA Server Framework  development model -</t>
   </si>
   <si>
@@ -314,17 +306,20 @@
   </si>
   <si>
     <t>imart</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0_);\(0\)"/>
     <numFmt numFmtId="165" formatCode="0_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,7 +352,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,8 +383,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -399,72 +400,112 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -472,29 +513,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -513,9 +534,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -534,12 +552,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -549,19 +561,58 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -858,853 +909,852 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="5.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="12.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="2" customWidth="1"/>
-    <col min="10" max="256" width="3.6640625" style="2" customWidth="1"/>
-    <col min="257" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" style="1" customWidth="1"/>
+    <col min="4" max="9" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11" max="257" width="3.7109375" style="1" customWidth="1"/>
+    <col min="258" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="41.25" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="2:10" ht="20.100000000000001" hidden="1" customHeight="1"/>
+    <row r="2" spans="2:10" ht="20.100000000000001" hidden="1" customHeight="1"/>
+    <row r="3" spans="2:10" ht="20.100000000000001" hidden="1" customHeight="1"/>
+    <row r="4" spans="2:10" ht="20.100000000000001" customHeight="1" thickBot="1"/>
+    <row r="5" spans="2:10" ht="45" customHeight="1" thickBot="1">
+      <c r="B5" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C5" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D5" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E5" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F5" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G5" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I5" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J5" s="28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="4">
+    <row r="6" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B6" s="20">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D6" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E6" s="20">
         <v>1000</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="4">
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="20">
         <v>1000</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I6" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J6" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="4">
+    <row r="7" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B7" s="20">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C7" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D7" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E7" s="20">
         <v>4000</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="4">
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="20">
         <v>4000</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I7" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J7" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="4">
+    <row r="8" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B8" s="20">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C8" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E8" s="20">
         <v>1000</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="4">
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="20">
         <v>1000</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I8" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J8" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="4">
+    <row r="9" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B9" s="20">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C9" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5">
+      <c r="E9" s="20"/>
+      <c r="F9" s="23">
         <v>30</v>
       </c>
-      <c r="F6" s="5">
+      <c r="G9" s="23">
         <v>10</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H9" s="20">
         <v>42</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I9" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J9" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="4">
+    <row r="10" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B10" s="20">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C10" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D10" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E10" s="20">
         <v>10</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="4">
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="20">
         <v>10</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7" t="s">
+      <c r="I10" s="24"/>
+      <c r="J10" s="25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="4">
+    <row r="11" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B11" s="20">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C11" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D11" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5">
+      <c r="E11" s="20"/>
+      <c r="F11" s="23">
         <v>30</v>
       </c>
-      <c r="F8" s="5">
+      <c r="G11" s="23">
         <v>10</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H11" s="20">
         <v>42</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I11" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="J11" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="4">
+    <row r="12" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B12" s="20">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D12" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E12" s="20">
         <v>10</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="4">
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="20">
         <v>10</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7" t="s">
+      <c r="I12" s="24"/>
+      <c r="J12" s="25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="4">
+    <row r="13" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B13" s="20">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C13" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D13" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E13" s="20">
         <v>4000</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="4">
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="20">
         <v>4000</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7" t="s">
+      <c r="I13" s="24"/>
+      <c r="J13" s="25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="4">
+    <row r="14" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B14" s="20">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C14" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D14" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E14" s="20">
         <v>50</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="4">
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="20">
         <v>50</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7" t="s">
+      <c r="I14" s="24"/>
+      <c r="J14" s="25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="4">
+    <row r="15" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B15" s="20">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C15" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D15" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E15" s="20">
         <v>50</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="4">
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="20">
         <v>50</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7" t="s">
+      <c r="I15" s="24"/>
+      <c r="J15" s="25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="4">
+    <row r="16" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B16" s="20">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C16" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D16" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E16" s="20">
         <v>50</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="4">
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="20">
         <v>50</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7" t="s">
+      <c r="I16" s="24"/>
+      <c r="J16" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="4">
+    <row r="17" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B17" s="20">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C17" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D17" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="4">
+      <c r="E17" s="20">
         <v>50</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="4">
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="20">
         <v>50</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7" t="s">
+      <c r="I17" s="24"/>
+      <c r="J17" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="4">
+    <row r="18" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B18" s="20">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C18" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D18" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="4">
+      <c r="E18" s="20">
         <v>4000</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="4">
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="20">
         <v>4000</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="7" t="s">
+      <c r="I18" s="24"/>
+      <c r="J18" s="25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="4">
+    <row r="19" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B19" s="20">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C19" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D19" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E19" s="20">
         <v>50</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="4">
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="20">
         <v>50</v>
       </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="7" t="s">
+      <c r="I19" s="24"/>
+      <c r="J19" s="25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="4">
+    <row r="20" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B20" s="20">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C20" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D20" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="4">
+      <c r="E20" s="20">
         <v>50</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="4">
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="20">
         <v>50</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="7" t="s">
+      <c r="I20" s="24"/>
+      <c r="J20" s="25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="4">
+    <row r="21" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B21" s="20">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C21" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D21" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="4">
+      <c r="E21" s="20">
         <v>50</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="4">
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="20">
         <v>50</v>
       </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="7" t="s">
+      <c r="I21" s="24"/>
+      <c r="J21" s="25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="4">
+    <row r="22" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B22" s="20">
         <v>17</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C22" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D22" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="4">
+      <c r="E22" s="20">
         <v>500</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="4">
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="20">
         <v>500</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="7" t="s">
+      <c r="I22" s="24"/>
+      <c r="J22" s="25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="4">
+    <row r="23" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B23" s="20">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D23" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="4">
+      <c r="E23" s="20">
         <v>500</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="4">
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="20">
         <v>500</v>
       </c>
-      <c r="H20" s="6"/>
-      <c r="I20" s="7" t="s">
+      <c r="I23" s="24"/>
+      <c r="J23" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="4">
+    <row r="24" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B24" s="20">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C24" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D24" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="4">
+      <c r="E24" s="20"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="20">
         <v>10</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="7" t="s">
+      <c r="I24" s="24"/>
+      <c r="J24" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="4">
+    <row r="25" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B25" s="20">
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C25" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D25" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="4">
+      <c r="E25" s="20">
         <v>100</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="4">
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="20">
         <v>100</v>
       </c>
-      <c r="H22" s="6"/>
-      <c r="I22" s="7" t="s">
+      <c r="I25" s="24"/>
+      <c r="J25" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="4">
+    <row r="26" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B26" s="20">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C26" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D26" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="4">
+      <c r="E26" s="20"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="20">
         <v>10</v>
       </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="7" t="s">
+      <c r="I26" s="24"/>
+      <c r="J26" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="4">
+    <row r="27" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B27" s="20">
         <v>22</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C27" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D27" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="4">
+      <c r="E27" s="20">
         <v>100</v>
       </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="4">
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="20">
         <v>100</v>
       </c>
-      <c r="H24" s="6"/>
-      <c r="I24" s="7" t="s">
+      <c r="I27" s="24"/>
+      <c r="J27" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="4">
+    <row r="28" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B28" s="20">
         <v>23</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C28" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D28" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="4">
+      <c r="E28" s="20"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="20">
         <v>10</v>
       </c>
-      <c r="H25" s="6"/>
-      <c r="I25" s="7" t="s">
+      <c r="I28" s="24"/>
+      <c r="J28" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="4">
+    <row r="29" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B29" s="20">
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C29" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D29" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="4">
+      <c r="E29" s="20">
         <v>100</v>
       </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="4">
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="20">
         <v>100</v>
       </c>
-      <c r="H26" s="6"/>
-      <c r="I26" s="7" t="s">
+      <c r="I29" s="24"/>
+      <c r="J29" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="4">
+    <row r="30" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B30" s="20">
         <v>25</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C30" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D30" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="4">
+      <c r="E30" s="20"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="20">
         <v>10</v>
       </c>
-      <c r="H27" s="6"/>
-      <c r="I27" s="7" t="s">
+      <c r="I30" s="24"/>
+      <c r="J30" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="4">
+    <row r="31" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B31" s="20">
         <v>26</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C31" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D31" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="4">
+      <c r="E31" s="20">
         <v>4000</v>
       </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="4">
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="20">
         <v>4000</v>
       </c>
-      <c r="H28" s="6"/>
-      <c r="I28" s="7" t="s">
+      <c r="I31" s="24"/>
+      <c r="J31" s="25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="4">
+    <row r="32" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B32" s="20">
         <v>27</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C32" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D32" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5">
+      <c r="E32" s="20"/>
+      <c r="F32" s="23">
         <v>30</v>
       </c>
-      <c r="F29" s="5">
+      <c r="G32" s="23">
         <v>10</v>
       </c>
-      <c r="G29" s="4">
+      <c r="H32" s="20">
         <v>42</v>
       </c>
-      <c r="H29" s="6"/>
-      <c r="I29" s="7" t="s">
+      <c r="I32" s="24"/>
+      <c r="J32" s="25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="4">
+    <row r="33" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B33" s="20">
         <v>28</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C33" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D33" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="4">
+      <c r="E33" s="20">
         <v>4000</v>
       </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="4">
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="20">
         <v>4000</v>
       </c>
-      <c r="H30" s="6"/>
-      <c r="I30" s="7" t="s">
+      <c r="I33" s="24"/>
+      <c r="J33" s="25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="4">
+    <row r="34" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B34" s="20">
         <v>29</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C34" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D34" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="5">
+      <c r="E34" s="20"/>
+      <c r="F34" s="23">
         <v>30</v>
       </c>
-      <c r="F31" s="5">
+      <c r="G34" s="23">
         <v>10</v>
       </c>
-      <c r="G31" s="4">
+      <c r="H34" s="20">
         <v>42</v>
       </c>
-      <c r="H31" s="6"/>
-      <c r="I31" s="7" t="s">
+      <c r="I34" s="24"/>
+      <c r="J34" s="25" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:V4"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:V4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y35" sqref="Y35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="2" customWidth="1"/>
-    <col min="2" max="256" width="3.6640625" style="2" customWidth="1"/>
-    <col min="257" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2" max="256" width="3.7109375" style="1" customWidth="1"/>
+    <col min="257" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" s="9" customFormat="1" ht="20" customHeight="1">
-      <c r="B2" s="24" t="s">
+    <row r="2" spans="2:22" s="2" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="B2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-    </row>
-    <row r="3" spans="2:22" ht="20" customHeight="1">
-      <c r="B3" s="24" t="s">
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+    </row>
+    <row r="3" spans="2:22" ht="20.100000000000001" customHeight="1">
+      <c r="B3" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-    </row>
-    <row r="4" spans="2:22" s="9" customFormat="1" ht="20" customHeight="1">
-      <c r="B4" s="24" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+    </row>
+    <row r="4" spans="2:22" s="2" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="B4" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1716,434 +1766,445 @@
     <mergeCell ref="F3:V3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="17" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="10" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" style="10" customWidth="1"/>
-    <col min="6" max="7" width="40.6640625" style="9" customWidth="1"/>
-    <col min="8" max="256" width="3.6640625" style="9" customWidth="1"/>
-    <col min="257" max="16384" width="8.83203125" style="9"/>
+    <col min="1" max="1" width="3.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" style="9" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="3" customWidth="1"/>
+    <col min="6" max="7" width="40.7109375" style="2" customWidth="1"/>
+    <col min="8" max="256" width="3.7109375" style="2" customWidth="1"/>
+    <col min="257" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="20" customHeight="1">
-      <c r="B1" s="27" t="s">
+    <row r="3" spans="2:7" ht="20.100000000000001" customHeight="1">
+      <c r="B3" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="22" t="b">
+      <c r="C3" s="31"/>
+      <c r="D3" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="21"/>
-    </row>
-    <row r="2" spans="2:7" ht="20" customHeight="1">
-      <c r="B2" s="26" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="2:7" ht="20.100000000000001" customHeight="1">
+      <c r="B4" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C4" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26" t="s">
+      <c r="D4" s="31"/>
+      <c r="E4" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-    </row>
-    <row r="3" spans="2:7" ht="20" customHeight="1">
-      <c r="B3" s="26"/>
-      <c r="C3" s="13" t="s">
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+    </row>
+    <row r="5" spans="2:7" ht="20.100000000000001" customHeight="1">
+      <c r="B5" s="31"/>
+      <c r="C5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="D5" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F5" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G5" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="20" customHeight="1">
-      <c r="B4" s="17">
+    <row r="6" spans="2:7" ht="20.100000000000001" customHeight="1">
+      <c r="B6" s="30">
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D6" s="30">
         <v>0</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E6" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="20" customHeight="1">
-      <c r="B5" s="17">
+    <row r="7" spans="2:7" ht="20.100000000000001" customHeight="1">
+      <c r="B7" s="30">
         <v>2</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D7" s="30">
         <v>1</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E7" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="20" customHeight="1">
-      <c r="B6" s="17">
+    <row r="8" spans="2:7" ht="20.100000000000001" customHeight="1">
+      <c r="B8" s="30">
         <v>3</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D8" s="30">
         <v>2</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E8" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="20" customHeight="1">
-      <c r="B7" s="17">
+    <row r="9" spans="2:7" ht="20.100000000000001" customHeight="1">
+      <c r="B9" s="30">
         <v>4</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D9" s="30">
         <v>3</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E9" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="20" customHeight="1">
-      <c r="B8" s="17">
+    <row r="10" spans="2:7" ht="20.100000000000001" customHeight="1">
+      <c r="B10" s="30">
         <v>5</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D10" s="30">
         <v>4</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E10" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="20" customHeight="1">
-      <c r="B9" s="17">
+    <row r="11" spans="2:7" ht="20.100000000000001" customHeight="1">
+      <c r="B11" s="30">
         <v>6</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D11" s="30">
         <v>5</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E11" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="20" customHeight="1">
-      <c r="B10" s="17">
+    <row r="12" spans="2:7" ht="20.100000000000001" customHeight="1">
+      <c r="B12" s="30">
         <v>7</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D12" s="30">
         <v>6</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E12" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="20" customHeight="1">
-      <c r="B11" s="17">
+    <row r="13" spans="2:7" ht="20.100000000000001" customHeight="1">
+      <c r="B13" s="30">
         <v>8</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D13" s="30">
         <v>7</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E13" s="3" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:J15"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="28.5" style="2" customWidth="1"/>
-    <col min="9" max="9" width="27.83203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="49.83203125" style="2" customWidth="1"/>
-    <col min="11" max="256" width="5.6640625" style="2" customWidth="1"/>
-    <col min="257" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="49.85546875" style="1" customWidth="1"/>
+    <col min="11" max="256" width="5.7109375" style="1" customWidth="1"/>
+    <col min="257" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="20" customHeight="1">
-      <c r="C1" s="15" t="s">
+    <row r="2" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B2" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B3" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-    </row>
-    <row r="2" spans="2:10" ht="20" customHeight="1">
-      <c r="B2" s="26" t="s">
+      <c r="E3" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B4" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C4" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D4" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E4" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-    </row>
-    <row r="3" spans="2:10" ht="20" customHeight="1">
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="13" t="s">
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+    </row>
+    <row r="5" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F5" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H5" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I5" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J5" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="20" customHeight="1">
-      <c r="B4" s="19">
+    <row r="6" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B6" s="32">
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D6" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F6" s="4">
         <v>50</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H6" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="20" t="s">
+      <c r="I6" s="4"/>
+      <c r="J6" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="24">
-      <c r="B5" s="19">
+    <row r="7" spans="2:10" ht="27">
+      <c r="B7" s="32">
         <v>2</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C7" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D7" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E7" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F7" s="4">
         <v>50</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="20" t="s">
+      <c r="I7" s="4"/>
+      <c r="J7" s="12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="24">
-      <c r="B6" s="19">
+    <row r="8" spans="2:10" ht="27">
+      <c r="B8" s="32">
         <v>3</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F8" s="4">
         <v>50</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H8" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="20" t="s">
+      <c r="I8" s="4"/>
+      <c r="J8" s="12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="20" customHeight="1">
-      <c r="B7" s="19">
+    <row r="9" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B9" s="32">
         <v>4</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C9" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D9" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E9" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F9" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="20"/>
-    </row>
-    <row r="8" spans="2:10" ht="20" customHeight="1">
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9" spans="2:10" ht="20" customHeight="1">
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="2:10" ht="20" customHeight="1">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="2:10" ht="20" customHeight="1">
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-    </row>
-    <row r="12" spans="2:10" ht="20" customHeight="1">
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="13" spans="2:10" ht="20" customHeight="1">
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="2:10" ht="20.100000000000001" customHeight="1">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:J2"/>
+  <mergeCells count="8">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="G4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>